<commit_message>
Updated two point recombination for constant domain
</commit_message>
<xml_diff>
--- a/randomvsGEP_forrester.xlsx
+++ b/randomvsGEP_forrester.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rafael Stevenson\Desktop\Kuliah\Tesis S2\GEP_ForresterCase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97CF01AF-329C-48AB-A6C4-D3AD6EA91CF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA6703DA-24B8-456B-B239-F08BDFB45D15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-15852" yWindow="1056" windowWidth="13320" windowHeight="10392" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="14">
   <si>
     <t>Run</t>
   </si>
@@ -362,6 +362,9 @@
   </si>
   <si>
     <t>std</t>
+  </si>
+  <si>
+    <t>avg</t>
   </si>
 </sst>
 </file>
@@ -447,7 +450,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -455,6 +458,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -737,8 +741,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -746,6 +750,7 @@
     <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -787,6 +792,9 @@
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
+      <c r="G2">
+        <v>4.3752368436632096</v>
+      </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="1">
@@ -803,6 +811,9 @@
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
+      <c r="G3">
+        <v>5.97479203386664</v>
+      </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="1">
@@ -819,6 +830,9 @@
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
+      <c r="G4">
+        <v>4.3578215436221797</v>
+      </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="1">
@@ -835,6 +849,9 @@
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
+      <c r="G5">
+        <v>4.7639364742200003</v>
+      </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="1">
@@ -851,6 +868,9 @@
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
+      <c r="G6">
+        <v>5.3231455157841401</v>
+      </c>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="1">
@@ -867,6 +887,9 @@
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
+      <c r="G7">
+        <v>4.7706259259189201</v>
+      </c>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="1">
@@ -883,6 +906,9 @@
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
+      <c r="G8">
+        <v>4.7915272970510099</v>
+      </c>
     </row>
     <row r="9" spans="1:10">
       <c r="A9" s="1">
@@ -899,6 +925,9 @@
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
+      <c r="G9">
+        <v>6.2721294019230003</v>
+      </c>
     </row>
     <row r="10" spans="1:10">
       <c r="A10" s="1">
@@ -915,6 +944,9 @@
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
+      <c r="G10">
+        <v>2.6330709280583502</v>
+      </c>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="1">
@@ -931,6 +963,9 @@
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
+      <c r="G11">
+        <v>4.8594749257104999</v>
+      </c>
     </row>
     <row r="12" spans="1:10">
       <c r="A12" s="1">
@@ -947,6 +982,9 @@
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
+      <c r="G12">
+        <v>5.1239591146356602</v>
+      </c>
     </row>
     <row r="13" spans="1:10">
       <c r="A13" s="1">
@@ -963,6 +1001,9 @@
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
+      <c r="G13">
+        <v>4.9904284217985504</v>
+      </c>
     </row>
     <row r="14" spans="1:10">
       <c r="A14" s="1">
@@ -979,6 +1020,9 @@
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
+      <c r="G14">
+        <v>4.4244977269524499</v>
+      </c>
     </row>
     <row r="15" spans="1:10">
       <c r="A15" s="1">
@@ -995,6 +1039,9 @@
       </c>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
+      <c r="G15">
+        <v>4.6735203843150597</v>
+      </c>
     </row>
     <row r="16" spans="1:10">
       <c r="A16" s="1">
@@ -1011,8 +1058,11 @@
       </c>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
-    </row>
-    <row r="17" spans="1:6">
+      <c r="G16">
+        <v>3.8398291810622198</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -1027,8 +1077,11 @@
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
-    </row>
-    <row r="18" spans="1:6">
+      <c r="G17">
+        <v>5.5070072333014499</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -1043,8 +1096,11 @@
       </c>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
-    </row>
-    <row r="19" spans="1:6">
+      <c r="G18">
+        <v>5.5865282662361597</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -1059,8 +1115,11 @@
       </c>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
-    </row>
-    <row r="20" spans="1:6">
+      <c r="G19">
+        <v>6.28639013586338</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -1075,8 +1134,11 @@
       </c>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
-    </row>
-    <row r="21" spans="1:6">
+      <c r="G20">
+        <v>5.6079734105141101</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -1091,8 +1153,11 @@
       </c>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
-    </row>
-    <row r="22" spans="1:6">
+      <c r="G21">
+        <v>4.02169629786657</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -1107,8 +1172,11 @@
       </c>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
-    </row>
-    <row r="23" spans="1:6">
+      <c r="G22">
+        <v>4.6675419339577298</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
       <c r="A23" s="1" t="s">
         <v>3</v>
       </c>
@@ -1129,8 +1197,12 @@
         <v>#DIV/0!</v>
       </c>
       <c r="F23" s="1"/>
-    </row>
-    <row r="24" spans="1:6">
+      <c r="G23" s="5">
+        <f>AVERAGE(G2:G22)</f>
+        <v>4.8976729998248238</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
       <c r="A24" s="4" t="s">
         <v>12</v>
       </c>
@@ -1146,39 +1218,39 @@
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:7">
       <c r="B25" s="2"/>
       <c r="C25" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:7">
       <c r="C26" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:7">
       <c r="C27" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:7">
       <c r="D28" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:7">
       <c r="D29" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:7">
       <c r="D30" s="3" t="s">
         <v>8</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="E1:E24 G1:J1 B1:C24 D23:E24 B25">
+  <conditionalFormatting sqref="E1:E24 G1:J1 B1:C24 D23:E24 B25 G23">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
@@ -1190,7 +1262,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E24 B2:C24 D23:E24 B25">
+  <conditionalFormatting sqref="E2:E24 B2:C24 D23:E24 B25 G23">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -1202,7 +1274,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E24 B2:C24 D23:E24">
+  <conditionalFormatting sqref="E2:E24 B2:C24 D23:E24 G23">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -1214,7 +1286,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:C24 D23:E24">
+  <conditionalFormatting sqref="B2:C24 D23:E24 G23">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -1247,8 +1319,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDF0A1C1-D8C8-46B0-911C-390D8528B2D2}">
   <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1256,6 +1328,7 @@
     <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -1295,6 +1368,9 @@
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
+      <c r="G2">
+        <v>4.7661811403748002</v>
+      </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="1">
@@ -1309,6 +1385,9 @@
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
+      <c r="G3">
+        <v>3.6889770705816498</v>
+      </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="1">
@@ -1323,6 +1402,9 @@
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
+      <c r="G4">
+        <v>3.9850500558022799</v>
+      </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="1">
@@ -1337,6 +1419,9 @@
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
+      <c r="G5">
+        <v>5.5865282662361597</v>
+      </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="1">
@@ -1351,6 +1436,9 @@
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
+      <c r="G6">
+        <v>5.7270316797652496</v>
+      </c>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="1">
@@ -1365,6 +1453,9 @@
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
+      <c r="G7">
+        <v>6.3593930788771003</v>
+      </c>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="1">
@@ -1379,6 +1470,9 @@
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
+      <c r="G8">
+        <v>4.7517590639181204</v>
+      </c>
     </row>
     <row r="9" spans="1:10">
       <c r="A9" s="1">
@@ -1393,6 +1487,9 @@
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
+      <c r="G9">
+        <v>3.8484165323830899</v>
+      </c>
     </row>
     <row r="10" spans="1:10">
       <c r="A10" s="1">
@@ -1407,6 +1504,9 @@
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
+      <c r="G10">
+        <v>4.9941463527084302</v>
+      </c>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="1">
@@ -1421,6 +1521,9 @@
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
+      <c r="G11">
+        <v>4.7748773732339096</v>
+      </c>
     </row>
     <row r="12" spans="1:10">
       <c r="A12" s="1">
@@ -1435,6 +1538,9 @@
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
+      <c r="G12">
+        <v>5.7534105418664501</v>
+      </c>
     </row>
     <row r="13" spans="1:10">
       <c r="A13" s="1">
@@ -1449,6 +1555,9 @@
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
+      <c r="G13">
+        <v>6.3396209590620201</v>
+      </c>
     </row>
     <row r="14" spans="1:10">
       <c r="A14" s="1">
@@ -1463,6 +1572,9 @@
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
+      <c r="G14">
+        <v>5.1406598564854997</v>
+      </c>
     </row>
     <row r="15" spans="1:10">
       <c r="A15" s="1">
@@ -1477,6 +1589,9 @@
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
+      <c r="G15">
+        <v>4.7605108246884598</v>
+      </c>
     </row>
     <row r="16" spans="1:10">
       <c r="A16" s="1">
@@ -1491,8 +1606,11 @@
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
-    </row>
-    <row r="17" spans="1:6">
+      <c r="G16">
+        <v>5.1290648617885104</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -1505,8 +1623,11 @@
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
-    </row>
-    <row r="18" spans="1:6">
+      <c r="G17">
+        <v>7.8936876021786802</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -1519,8 +1640,11 @@
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
-    </row>
-    <row r="19" spans="1:6">
+      <c r="G18">
+        <v>6.8688831166988296</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -1533,8 +1657,11 @@
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
-    </row>
-    <row r="20" spans="1:6">
+      <c r="G19">
+        <v>4.74656203008945</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -1547,8 +1674,11 @@
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
-    </row>
-    <row r="21" spans="1:6">
+      <c r="G20">
+        <v>5.5122425841103002</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -1561,8 +1691,11 @@
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
-    </row>
-    <row r="22" spans="1:6">
+      <c r="G21">
+        <v>3.8945310711593502</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -1575,8 +1708,11 @@
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
-    </row>
-    <row r="23" spans="1:6">
+      <c r="G22">
+        <v>7.7712048030548102</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
       <c r="A23" s="1" t="s">
         <v>3</v>
       </c>
@@ -1590,9 +1726,15 @@
       </c>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-    </row>
-    <row r="24" spans="1:6">
+      <c r="F23" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G23">
+        <f>AVERAGE(G2:G22)</f>
+        <v>5.3472732792887214</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
       <c r="A24" t="s">
         <v>12</v>
       </c>
@@ -1605,18 +1747,25 @@
         <v>1.6128216492543037</v>
       </c>
       <c r="E24" s="2"/>
-    </row>
-    <row r="27" spans="1:6">
+      <c r="F24" t="s">
+        <v>12</v>
+      </c>
+      <c r="G24">
+        <f>_xlfn.STDEV.P(G2:G22)</f>
+        <v>1.1542973049599885</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
       <c r="D27" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:7">
       <c r="D28" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:7">
       <c r="D29" s="3" t="s">
         <v>8</v>
       </c>

</xml_diff>

<commit_message>
Updated two point recombination
</commit_message>
<xml_diff>
--- a/randomvsGEP_forrester.xlsx
+++ b/randomvsGEP_forrester.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rafael Stevenson\Desktop\Kuliah\Tesis S2\GEP_ForresterCase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA6703DA-24B8-456B-B239-F08BDFB45D15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5009B0B0-9869-4A3B-9C37-CABED14A609D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15852" yWindow="1056" windowWidth="13320" windowHeight="10392" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1 (2)" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1 (3)" sheetId="3" r:id="rId2"/>
+    <sheet name="Random Constants" sheetId="2" r:id="rId3"/>
+    <sheet name="Random Constants (2)" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="14">
   <si>
     <t>Run</t>
   </si>
@@ -741,8 +743,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I34" sqref="I34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1316,11 +1318,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDF0A1C1-D8C8-46B0-911C-390D8528B2D2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45436DD9-BF20-439A-ACBC-0DF56BCE860D}">
   <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1368,9 +1370,6 @@
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
-      <c r="G2">
-        <v>4.7661811403748002</v>
-      </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="1">
@@ -1385,9 +1384,6 @@
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
-      <c r="G3">
-        <v>3.6889770705816498</v>
-      </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="1">
@@ -1402,9 +1398,6 @@
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
-      <c r="G4">
-        <v>3.9850500558022799</v>
-      </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="1">
@@ -1419,9 +1412,6 @@
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
-      <c r="G5">
-        <v>5.5865282662361597</v>
-      </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="1">
@@ -1436,9 +1426,6 @@
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
-      <c r="G6">
-        <v>5.7270316797652496</v>
-      </c>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="1">
@@ -1453,9 +1440,6 @@
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
-      <c r="G7">
-        <v>6.3593930788771003</v>
-      </c>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="1">
@@ -1470,9 +1454,6 @@
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
-      <c r="G8">
-        <v>4.7517590639181204</v>
-      </c>
     </row>
     <row r="9" spans="1:10">
       <c r="A9" s="1">
@@ -1487,9 +1468,6 @@
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
-      <c r="G9">
-        <v>3.8484165323830899</v>
-      </c>
     </row>
     <row r="10" spans="1:10">
       <c r="A10" s="1">
@@ -1504,9 +1482,6 @@
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
-      <c r="G10">
-        <v>4.9941463527084302</v>
-      </c>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="1">
@@ -1521,9 +1496,6 @@
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
-      <c r="G11">
-        <v>4.7748773732339096</v>
-      </c>
     </row>
     <row r="12" spans="1:10">
       <c r="A12" s="1">
@@ -1538,9 +1510,6 @@
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
-      <c r="G12">
-        <v>5.7534105418664501</v>
-      </c>
     </row>
     <row r="13" spans="1:10">
       <c r="A13" s="1">
@@ -1555,9 +1524,6 @@
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
-      <c r="G13">
-        <v>6.3396209590620201</v>
-      </c>
     </row>
     <row r="14" spans="1:10">
       <c r="A14" s="1">
@@ -1572,9 +1538,6 @@
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
-      <c r="G14">
-        <v>5.1406598564854997</v>
-      </c>
     </row>
     <row r="15" spans="1:10">
       <c r="A15" s="1">
@@ -1589,9 +1552,6 @@
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
-      <c r="G15">
-        <v>4.7605108246884598</v>
-      </c>
     </row>
     <row r="16" spans="1:10">
       <c r="A16" s="1">
@@ -1606,9 +1566,6 @@
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
-      <c r="G16">
-        <v>5.1290648617885104</v>
-      </c>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="1">
@@ -1623,9 +1580,6 @@
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
-      <c r="G17">
-        <v>7.8936876021786802</v>
-      </c>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="1">
@@ -1640,9 +1594,6 @@
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
-      <c r="G18">
-        <v>6.8688831166988296</v>
-      </c>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="1">
@@ -1657,9 +1608,6 @@
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
-      <c r="G19">
-        <v>4.74656203008945</v>
-      </c>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="1">
@@ -1674,9 +1622,6 @@
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
-      <c r="G20">
-        <v>5.5122425841103002</v>
-      </c>
     </row>
     <row r="21" spans="1:7">
       <c r="A21" s="1">
@@ -1691,9 +1636,6 @@
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
-      <c r="G21">
-        <v>3.8945310711593502</v>
-      </c>
     </row>
     <row r="22" spans="1:7">
       <c r="A22" s="1">
@@ -1708,9 +1650,6 @@
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
-      <c r="G22">
-        <v>7.7712048030548102</v>
-      </c>
     </row>
     <row r="23" spans="1:7">
       <c r="A23" s="1" t="s">
@@ -1729,9 +1668,9 @@
       <c r="F23" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G23">
+      <c r="G23" t="e">
         <f>AVERAGE(G2:G22)</f>
-        <v>5.3472732792887214</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -1750,9 +1689,467 @@
       <c r="F24" t="s">
         <v>12</v>
       </c>
-      <c r="G24">
+      <c r="G24" t="e">
         <f>_xlfn.STDEV.P(G2:G22)</f>
-        <v>1.1542973049599885</v>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="D27" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="D28" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="D29" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="E1:E24 G1:J1 D23 B1:C24">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2:E24 D23 B2:C24">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2:E23 B2:C23 D23">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:C23 D23:E23">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:C23">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDF0A1C1-D8C8-46B0-911C-390D8528B2D2}">
+  <dimension ref="A1:J29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>5.0548234896958997</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0.54453311395474002</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>6.06956988808642</v>
+      </c>
+      <c r="C3" s="1">
+        <v>3.83433090897771</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>5.9465904766228901</v>
+      </c>
+      <c r="C4" s="1">
+        <v>5.6807064123942297</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1">
+        <v>5.7494851893358998</v>
+      </c>
+      <c r="C5" s="1">
+        <v>5.7188920732689104</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1">
+        <v>4.6364527702584102</v>
+      </c>
+      <c r="C6" s="1">
+        <v>4.3322203029670501</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1">
+        <v>4.7880520722257396</v>
+      </c>
+      <c r="C7" s="1">
+        <v>6.5415247455265</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1">
+        <v>7.2540423201702096</v>
+      </c>
+      <c r="C8" s="1">
+        <v>10.930615830765401</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1">
+        <v>5.46629008304342</v>
+      </c>
+      <c r="C9" s="1">
+        <v>4.7566786898670497</v>
+      </c>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1">
+        <v>5.2249617106738002</v>
+      </c>
+      <c r="C10" s="1">
+        <v>4.7490863527397202</v>
+      </c>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1">
+        <v>3.3512478572444002</v>
+      </c>
+      <c r="C11" s="1">
+        <v>6.52742548015945</v>
+      </c>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1">
+        <v>4.5485029129541097</v>
+      </c>
+      <c r="C12" s="1">
+        <v>8.5661168339770803</v>
+      </c>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1">
+        <v>4.7755181171133101</v>
+      </c>
+      <c r="C13" s="1">
+        <v>3.8806767344436999</v>
+      </c>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1">
+        <v>5.8240192721003003</v>
+      </c>
+      <c r="C14" s="1">
+        <v>0.52219643729961396</v>
+      </c>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1">
+        <v>4.9880629468935096</v>
+      </c>
+      <c r="C15" s="1">
+        <v>5.54793833356901</v>
+      </c>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16" s="1">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1">
+        <v>6.38867281553176</v>
+      </c>
+      <c r="C16" s="1">
+        <v>4.8307124377977901</v>
+      </c>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="1">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1">
+        <v>6.80505251417922</v>
+      </c>
+      <c r="C17" s="1">
+        <v>4.7580544023353797</v>
+      </c>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="1">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1">
+        <v>7.0139954817328496</v>
+      </c>
+      <c r="C18" s="1">
+        <v>4.78049755251826</v>
+      </c>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" s="1">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1">
+        <v>5.5458454174790504</v>
+      </c>
+      <c r="C19" s="1">
+        <v>7.2120121318486001</v>
+      </c>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" s="1">
+        <v>19</v>
+      </c>
+      <c r="B20" s="1">
+        <v>7.0821978453152301</v>
+      </c>
+      <c r="C20" s="1">
+        <v>4.7827261278749997</v>
+      </c>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" s="1">
+        <v>20</v>
+      </c>
+      <c r="B21" s="1">
+        <v>6.61534445704656</v>
+      </c>
+      <c r="C21" s="1">
+        <v>4.8021429018701296</v>
+      </c>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" s="1">
+        <v>21</v>
+      </c>
+      <c r="B22" s="1">
+        <v>5.2574110570190404</v>
+      </c>
+      <c r="C22" s="1">
+        <v>1.8304638819049801</v>
+      </c>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23" s="1">
+        <f>AVERAGE(B2:B22)</f>
+        <v>5.637435175939145</v>
+      </c>
+      <c r="C23" s="1">
+        <f>AVERAGE(C2:C22)</f>
+        <v>5.0061691279076319</v>
+      </c>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G23" t="e">
+        <f>AVERAGE(G2:G22)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" t="s">
+        <v>12</v>
+      </c>
+      <c r="B24" s="2">
+        <f>_xlfn.STDEV.P(B2:B22)</f>
+        <v>0.97104396967437245</v>
+      </c>
+      <c r="C24" s="2">
+        <f>_xlfn.STDEV.P(C2:C22)</f>
+        <v>2.3106449919426244</v>
+      </c>
+      <c r="E24" s="2"/>
+      <c r="F24" t="s">
+        <v>12</v>
+      </c>
+      <c r="G24" t="e">
+        <f>_xlfn.STDEV.P(G2:G22)</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -1834,4 +2231,462 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE6291EE-0FAB-4D5D-B45F-B894B16AFF1C}">
+  <dimension ref="A1:J29"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>2.7835216246358598</v>
+      </c>
+      <c r="C2" s="1">
+        <v>5.5865282662361597</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1.1830009991995301</v>
+      </c>
+      <c r="C3" s="1">
+        <v>5.3972219661340404</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>4.71150336148688</v>
+      </c>
+      <c r="C4" s="1">
+        <v>5.5865282662361597</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1">
+        <v>5.0895393881448303</v>
+      </c>
+      <c r="C5" s="1">
+        <v>6.6864925056735398</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1">
+        <v>5.7041645419642197</v>
+      </c>
+      <c r="C6" s="1">
+        <v>8.6778406022589607</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1">
+        <v>4.7063232298589499</v>
+      </c>
+      <c r="C7" s="1">
+        <v>1.4635238296940101</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1">
+        <v>4.8936718799632697</v>
+      </c>
+      <c r="C8" s="1">
+        <v>3.9098782579126499</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1">
+        <v>3.0683018650204499</v>
+      </c>
+      <c r="C9" s="1">
+        <v>6.7431201895949702</v>
+      </c>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1">
+        <v>5.3264537433935804</v>
+      </c>
+      <c r="C10" s="1">
+        <v>4.6194924935743398</v>
+      </c>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1">
+        <v>3.6005796143265001</v>
+      </c>
+      <c r="C11" s="1">
+        <v>4.5301193499602999</v>
+      </c>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1">
+        <v>4.8445184807710602</v>
+      </c>
+      <c r="C12" s="1">
+        <v>5.9978785808366197</v>
+      </c>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1">
+        <v>5.0963066011460496</v>
+      </c>
+      <c r="C13" s="1">
+        <v>4.1336580069993998</v>
+      </c>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1">
+        <v>4.1670949202168703</v>
+      </c>
+      <c r="C14" s="1">
+        <v>4.7564610394950604</v>
+      </c>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1">
+        <v>4.0095677842067099</v>
+      </c>
+      <c r="C15" s="1">
+        <v>0.59604982210183399</v>
+      </c>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16" s="1">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1">
+        <v>5.8760602995276399</v>
+      </c>
+      <c r="C16" s="1">
+        <v>4.8417983665537996</v>
+      </c>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="1">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1">
+        <v>4.4891627443656201</v>
+      </c>
+      <c r="C17" s="1">
+        <v>7.6281809061580601</v>
+      </c>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="1">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1">
+        <v>5.3416314092462898</v>
+      </c>
+      <c r="C18" s="1">
+        <v>1.40996813637536</v>
+      </c>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" s="1">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1">
+        <v>4.9677226689839999</v>
+      </c>
+      <c r="C19" s="1">
+        <v>5.3258963654136497</v>
+      </c>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" s="1">
+        <v>19</v>
+      </c>
+      <c r="B20" s="1">
+        <v>2.1370402222328999</v>
+      </c>
+      <c r="C20" s="1">
+        <v>4.4798336072940597</v>
+      </c>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" s="1">
+        <v>20</v>
+      </c>
+      <c r="B21" s="1">
+        <v>5.5048490774587897</v>
+      </c>
+      <c r="C21" s="1">
+        <v>7.0344393313582199</v>
+      </c>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" s="1">
+        <v>21</v>
+      </c>
+      <c r="B22" s="1">
+        <v>6.0890301823830804</v>
+      </c>
+      <c r="C22" s="1">
+        <v>5.8071729403276304</v>
+      </c>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23" s="1">
+        <f>AVERAGE(B2:B22)</f>
+        <v>4.4566687923110981</v>
+      </c>
+      <c r="C23" s="1">
+        <f>AVERAGE(C2:C22)</f>
+        <v>5.0100991823899435</v>
+      </c>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G23" t="e">
+        <f>AVERAGE(G2:G22)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" t="s">
+        <v>12</v>
+      </c>
+      <c r="B24" s="2">
+        <f>_xlfn.STDEV.P(B2:B22)</f>
+        <v>1.2393479782502346</v>
+      </c>
+      <c r="C24" s="2">
+        <f>_xlfn.STDEV.P(C2:C22)</f>
+        <v>1.9579125982847188</v>
+      </c>
+      <c r="E24" s="2"/>
+      <c r="F24" t="s">
+        <v>12</v>
+      </c>
+      <c r="G24" t="e">
+        <f>_xlfn.STDEV.P(G2:G22)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="D27" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="D28" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="D29" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="E1:E24 G1:J1 D23 B1:C24">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2:E24 D23 B2:C24">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2:E23 B2:C23 D23">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:C23 D23:E23">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:C23">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Tried various one point but no better results
</commit_message>
<xml_diff>
--- a/randomvsGEP_forrester.xlsx
+++ b/randomvsGEP_forrester.xlsx
@@ -8,37 +8,39 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rafael Stevenson\Desktop\Kuliah\Tesis S2\GEP_ForresterCase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A4185C4-E955-46AA-806E-A823A8B36502}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1382B309-616A-416D-BD30-046772F56581}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1 (3)" sheetId="3" r:id="rId2"/>
     <sheet name="Rand Cons pop250, gen100" sheetId="2" r:id="rId3"/>
     <sheet name="Rand Cons pop300, gen200" sheetId="4" r:id="rId4"/>
+    <sheet name="edited onepoint recomb" sheetId="5" r:id="rId5"/>
+    <sheet name="Rand Cons pop250, gen100 (2)" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$B$1</definedName>
     <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$B$2:$B$22</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">'Sheet1 (3)'!$C$1</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">'Sheet1 (3)'!$C$2:$C$22</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">'Rand Cons pop250, gen100'!$B$1</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">'Rand Cons pop250, gen100'!$B$2:$B$22</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">'Rand Cons pop250, gen100'!$C$1</definedName>
-    <definedName name="_xlchart.v1.15" hidden="1">'Rand Cons pop250, gen100'!$C$2:$C$22</definedName>
-    <definedName name="_xlchart.v1.16" hidden="1">'Rand Cons pop300, gen200'!$B$1</definedName>
-    <definedName name="_xlchart.v1.17" hidden="1">'Rand Cons pop300, gen200'!$B$2:$B$22</definedName>
-    <definedName name="_xlchart.v1.18" hidden="1">'Rand Cons pop300, gen200'!$C$1</definedName>
-    <definedName name="_xlchart.v1.19" hidden="1">'Rand Cons pop300, gen200'!$C$2:$C$22</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">'Rand Cons pop250, gen100'!$C$1</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">'Rand Cons pop250, gen100'!$C$2:$C$22</definedName>
+    <definedName name="_xlchart.v1.12" hidden="1">'Rand Cons pop300, gen200'!$B$1</definedName>
+    <definedName name="_xlchart.v1.13" hidden="1">'Rand Cons pop300, gen200'!$B$2:$B$22</definedName>
+    <definedName name="_xlchart.v1.14" hidden="1">'Rand Cons pop300, gen200'!$C$1</definedName>
+    <definedName name="_xlchart.v1.15" hidden="1">'Rand Cons pop300, gen200'!$C$2:$C$22</definedName>
+    <definedName name="_xlchart.v1.16" hidden="1">'Rand Cons pop250, gen100 (2)'!$B$1</definedName>
+    <definedName name="_xlchart.v1.17" hidden="1">'Rand Cons pop250, gen100 (2)'!$B$2:$B$22</definedName>
+    <definedName name="_xlchart.v1.18" hidden="1">'Rand Cons pop250, gen100 (2)'!$C$1</definedName>
+    <definedName name="_xlchart.v1.19" hidden="1">'Rand Cons pop250, gen100 (2)'!$C$2:$C$22</definedName>
     <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$C$1</definedName>
     <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$C$2:$C$22</definedName>
     <definedName name="_xlchart.v1.4" hidden="1">'Sheet1 (3)'!$B$1</definedName>
     <definedName name="_xlchart.v1.5" hidden="1">'Sheet1 (3)'!$B$2:$B$22</definedName>
     <definedName name="_xlchart.v1.6" hidden="1">'Sheet1 (3)'!$C$1</definedName>
     <definedName name="_xlchart.v1.7" hidden="1">'Sheet1 (3)'!$C$2:$C$22</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">'Sheet1 (3)'!$B$1</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">'Sheet1 (3)'!$B$2:$B$22</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">'Rand Cons pop250, gen100'!$B$1</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">'Rand Cons pop250, gen100'!$B$2:$B$22</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -60,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="24">
   <si>
     <t>Run</t>
   </si>
@@ -411,6 +413,15 @@
   <si>
     <t>Max</t>
   </si>
+  <si>
+    <t>with one point recomb modif</t>
+  </si>
+  <si>
+    <t>one point sederhana</t>
+  </si>
+  <si>
+    <t>one point simple with recom index whole to dc</t>
+  </si>
 </sst>
 </file>
 
@@ -449,12 +460,18 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -495,7 +512,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -504,6 +521,8 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -586,12 +605,12 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.9</cx:f>
+        <cx:f>_xlchart.v1.5</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.11</cx:f>
+        <cx:f>_xlchart.v1.7</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -602,7 +621,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{D4842B8D-3E64-48D7-99E1-1FCDF8CFF0B2}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.8</cx:f>
+              <cx:f>_xlchart.v1.4</cx:f>
               <cx:v>Random (25000)</cx:v>
             </cx:txData>
           </cx:tx>
@@ -615,7 +634,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{59BC2FA5-6C8C-4EE6-B8B7-B81E827F736F}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.10</cx:f>
+              <cx:f>_xlchart.v1.6</cx:f>
               <cx:v>GEP(pop250, gen100)</cx:v>
             </cx:txData>
           </cx:tx>
@@ -645,12 +664,12 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.13</cx:f>
+        <cx:f>_xlchart.v1.9</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.15</cx:f>
+        <cx:f>_xlchart.v1.11</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -661,7 +680,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{4F46B704-B8A4-4ED1-9E0D-9BCF24C93E6E}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.12</cx:f>
+              <cx:f>_xlchart.v1.8</cx:f>
               <cx:v>Random (25000)</cx:v>
             </cx:txData>
           </cx:tx>
@@ -674,7 +693,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{2EEC4223-537A-4785-85C6-06056A116479}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.14</cx:f>
+              <cx:f>_xlchart.v1.10</cx:f>
               <cx:v>GEP(pop250, gen100)</cx:v>
             </cx:txData>
           </cx:tx>
@@ -705,6 +724,66 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
+        <cx:f>_xlchart.v1.13</cx:f>
+      </cx:numDim>
+    </cx:data>
+    <cx:data id="1">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.15</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0"/>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="boxWhisker" uniqueId="{87A0E5C1-60BE-48A8-BD9A-1C0C30990759}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.12</cx:f>
+              <cx:v>Random (60000)</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="0"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+        <cx:series layoutId="boxWhisker" uniqueId="{FBE50CB1-B5F1-4CE8-9936-B286058E83BD}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.14</cx:f>
+              <cx:v>GEP(pop300, gen200)</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="1"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+      </cx:plotAreaRegion>
+      <cx:axis id="0">
+        <cx:catScaling gapWidth="1"/>
+        <cx:tickLabels/>
+      </cx:axis>
+      <cx:axis id="1">
+        <cx:valScaling/>
+        <cx:majorGridlines/>
+        <cx:tickLabels/>
+      </cx:axis>
+    </cx:plotArea>
+    <cx:legend pos="t" align="ctr" overlay="0"/>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
+<file path=xl/charts/chartEx5.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:numDim type="val">
         <cx:f>_xlchart.v1.17</cx:f>
       </cx:numDim>
     </cx:data>
@@ -718,11 +797,11 @@
     <cx:title pos="t" align="ctr" overlay="0"/>
     <cx:plotArea>
       <cx:plotAreaRegion>
-        <cx:series layoutId="boxWhisker" uniqueId="{87A0E5C1-60BE-48A8-BD9A-1C0C30990759}">
+        <cx:series layoutId="boxWhisker" uniqueId="{4F46B704-B8A4-4ED1-9E0D-9BCF24C93E6E}">
           <cx:tx>
             <cx:txData>
               <cx:f>_xlchart.v1.16</cx:f>
-              <cx:v>Random (60000)</cx:v>
+              <cx:v>Random (25000)</cx:v>
             </cx:txData>
           </cx:tx>
           <cx:dataId val="0"/>
@@ -731,11 +810,11 @@
             <cx:statistics quartileMethod="exclusive"/>
           </cx:layoutPr>
         </cx:series>
-        <cx:series layoutId="boxWhisker" uniqueId="{FBE50CB1-B5F1-4CE8-9936-B286058E83BD}">
+        <cx:series layoutId="boxWhisker" uniqueId="{2EEC4223-537A-4785-85C6-06056A116479}">
           <cx:tx>
             <cx:txData>
               <cx:f>_xlchart.v1.18</cx:f>
-              <cx:v>GEP(pop300, gen200)</cx:v>
+              <cx:v>GEP(pop250, gen100)</cx:v>
             </cx:txData>
           </cx:tx>
           <cx:dataId val="1"/>
@@ -920,6 +999,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="406">
   <cs:axisTitle>
@@ -2466,6 +2585,521 @@
 </file>
 
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="406">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="406">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3312,6 +3946,89 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>581024</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>123824</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="2" name="Chart 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9C50A7B4-6ED1-4450-9607-AEED3F01B1DA}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="11010899" y="1457324"/>
+              <a:ext cx="4010026" cy="3038476"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100"/>
+                <a:t>This chart isn't available in your version of Excel.
+Editing this shape or saving this workbook into a different file format will permanently break the chart.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -4615,7 +5332,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDF0A1C1-D8C8-46B0-911C-390D8528B2D2}">
   <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="R12" sqref="R12"/>
     </sheetView>
   </sheetViews>
@@ -5562,4 +6279,763 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1261C2F2-2AE7-4EDD-A179-1112E73B1946}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39C6E40D-A913-438D-95D9-50A6F5CDBA8C}">
+  <dimension ref="A1:R29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="Q1" t="s">
+        <v>14</v>
+      </c>
+      <c r="R1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>5.0548234896958997</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0.54453311395474002</v>
+      </c>
+      <c r="D2" s="1">
+        <v>4.2063511006070602</v>
+      </c>
+      <c r="E2" s="1">
+        <v>3.9149591849411598</v>
+      </c>
+      <c r="F2" s="1">
+        <v>5.6789720582986396</v>
+      </c>
+      <c r="G2">
+        <v>5.5865282662361597</v>
+      </c>
+      <c r="P2" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q2">
+        <f>MIN(B2:B22)</f>
+        <v>3.3512478572444002</v>
+      </c>
+      <c r="R2">
+        <f>MIN(C2:C22)</f>
+        <v>0.52219643729961396</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>6.06956988808642</v>
+      </c>
+      <c r="C3" s="1">
+        <v>3.83433090897771</v>
+      </c>
+      <c r="D3" s="1">
+        <v>9.6596095845675194</v>
+      </c>
+      <c r="E3" s="1">
+        <v>4.4798517670645603</v>
+      </c>
+      <c r="F3" s="1">
+        <v>4.2893699873453501</v>
+      </c>
+      <c r="G3">
+        <v>4.0582233106820702</v>
+      </c>
+      <c r="P3" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q3">
+        <f>_xlfn.QUARTILE.INC(B2:B22,1)</f>
+        <v>4.9880629468935096</v>
+      </c>
+      <c r="R3">
+        <f>_xlfn.QUARTILE.INC(C2:C22,1)</f>
+        <v>4.3322203029670501</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>5.9465904766228901</v>
+      </c>
+      <c r="C4" s="1">
+        <v>5.6807064123942297</v>
+      </c>
+      <c r="D4" s="1">
+        <v>6.5306567817188403</v>
+      </c>
+      <c r="E4" s="1">
+        <v>5.6083373609446898</v>
+      </c>
+      <c r="F4" s="1">
+        <v>7.0559338615553999</v>
+      </c>
+      <c r="G4">
+        <v>4.8040735588063299</v>
+      </c>
+      <c r="P4" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q4">
+        <f>_xlfn.QUARTILE.INC(B2:B22,2)</f>
+        <v>5.5458454174790504</v>
+      </c>
+      <c r="R4">
+        <f>_xlfn.QUARTILE.INC(C2:C22,2)</f>
+        <v>4.7827261278749997</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1">
+        <v>5.7494851893358998</v>
+      </c>
+      <c r="C5" s="1">
+        <v>5.7188920732689104</v>
+      </c>
+      <c r="D5" s="1">
+        <v>5.1302132134931302</v>
+      </c>
+      <c r="E5" s="1">
+        <v>5.0484514606359596</v>
+      </c>
+      <c r="F5" s="1">
+        <v>8.9099156699200801</v>
+      </c>
+      <c r="G5">
+        <v>5.6414402855879997</v>
+      </c>
+      <c r="P5" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q5">
+        <f>_xlfn.QUARTILE.INC(B2:B22,3)</f>
+        <v>6.38867281553176</v>
+      </c>
+      <c r="R5">
+        <f>_xlfn.QUARTILE.INC(C2:C22,3)</f>
+        <v>5.7188920732689104</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1">
+        <v>4.6364527702584102</v>
+      </c>
+      <c r="C6" s="1">
+        <v>4.3322203029670501</v>
+      </c>
+      <c r="D6" s="1">
+        <v>4.7605510592801101</v>
+      </c>
+      <c r="E6" s="1">
+        <v>5.0160544204140498</v>
+      </c>
+      <c r="F6" s="1">
+        <v>7.6316923527704397</v>
+      </c>
+      <c r="G6">
+        <v>4.72630118266986</v>
+      </c>
+      <c r="P6" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q6">
+        <f>MAX(B2:B22)</f>
+        <v>7.2540423201702096</v>
+      </c>
+      <c r="R6">
+        <f>MAX(C2:C22)</f>
+        <v>10.930615830765401</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1">
+        <v>4.7880520722257396</v>
+      </c>
+      <c r="C7" s="1">
+        <v>6.5415247455265</v>
+      </c>
+      <c r="D7" s="1">
+        <v>5.9147651837478303</v>
+      </c>
+      <c r="E7" s="1">
+        <v>5.7031625263843102</v>
+      </c>
+      <c r="F7" s="1">
+        <v>3.23885825369628</v>
+      </c>
+      <c r="G7">
+        <v>4.42549218233101</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1">
+        <v>7.2540423201702096</v>
+      </c>
+      <c r="C8" s="1">
+        <v>10.930615830765401</v>
+      </c>
+      <c r="D8" s="1">
+        <v>6.6645017885470503</v>
+      </c>
+      <c r="E8" s="1">
+        <v>4.9109843051945399</v>
+      </c>
+      <c r="F8" s="1">
+        <v>6.3163250307737098</v>
+      </c>
+      <c r="G8">
+        <v>4.5949799283728696</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1">
+        <v>5.46629008304342</v>
+      </c>
+      <c r="C9" s="1">
+        <v>4.7566786898670497</v>
+      </c>
+      <c r="D9" s="1">
+        <v>4.7586927393565999</v>
+      </c>
+      <c r="E9" s="1">
+        <v>7.7861930599358002</v>
+      </c>
+      <c r="F9" s="1">
+        <v>4.1228806539280498</v>
+      </c>
+      <c r="G9">
+        <v>6.3125992807620701</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1">
+        <v>5.2249617106738002</v>
+      </c>
+      <c r="C10" s="1">
+        <v>4.7490863527397202</v>
+      </c>
+      <c r="D10" s="1">
+        <v>5.6414402855879997</v>
+      </c>
+      <c r="E10" s="1">
+        <v>4.3614559594822202</v>
+      </c>
+      <c r="F10" s="1">
+        <v>5.6178265715912499</v>
+      </c>
+      <c r="G10">
+        <v>5.5231815257180603</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1">
+        <v>3.3512478572444002</v>
+      </c>
+      <c r="C11" s="1">
+        <v>6.52742548015945</v>
+      </c>
+      <c r="D11" s="1">
+        <v>1.69987661844368</v>
+      </c>
+      <c r="E11" s="1">
+        <v>4.1609519665725303</v>
+      </c>
+      <c r="F11" s="1">
+        <v>4.5354001948767797</v>
+      </c>
+      <c r="G11">
+        <v>7.33620776081065</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1">
+        <v>4.5485029129541097</v>
+      </c>
+      <c r="C12" s="1">
+        <v>8.5661168339770803</v>
+      </c>
+      <c r="D12" s="1">
+        <v>5.7245641668384204</v>
+      </c>
+      <c r="E12" s="1">
+        <v>4.73772188318926</v>
+      </c>
+      <c r="F12" s="1">
+        <v>4.8516864342063402</v>
+      </c>
+      <c r="G12">
+        <v>5.1624527578368502</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1">
+        <v>4.7755181171133101</v>
+      </c>
+      <c r="C13" s="1">
+        <v>3.8806767344436999</v>
+      </c>
+      <c r="D13" s="1">
+        <v>6.8415773252661696</v>
+      </c>
+      <c r="E13" s="1">
+        <v>5.51976720255493</v>
+      </c>
+      <c r="F13" s="1">
+        <v>5.2391795743912102</v>
+      </c>
+      <c r="G13">
+        <v>4.35874534523085</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1">
+        <v>5.8240192721003003</v>
+      </c>
+      <c r="C14" s="1">
+        <v>0.52219643729961396</v>
+      </c>
+      <c r="D14" s="1">
+        <v>5.1154528253458</v>
+      </c>
+      <c r="E14" s="1">
+        <v>4.7390715884199599</v>
+      </c>
+      <c r="F14" s="1">
+        <v>8.7819417221141194</v>
+      </c>
+      <c r="G14">
+        <v>4.8175500647658298</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1">
+        <v>4.9880629468935096</v>
+      </c>
+      <c r="C15" s="1">
+        <v>5.54793833356901</v>
+      </c>
+      <c r="D15" s="1">
+        <v>1.2821016154678</v>
+      </c>
+      <c r="E15" s="1">
+        <v>9.0753860896416292</v>
+      </c>
+      <c r="F15" s="1">
+        <v>1.7566222820158099</v>
+      </c>
+      <c r="G15">
+        <v>8.8406261722071307</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18">
+      <c r="A16" s="1">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1">
+        <v>6.38867281553176</v>
+      </c>
+      <c r="C16" s="1">
+        <v>4.8307124377977901</v>
+      </c>
+      <c r="D16" s="1">
+        <v>6.07435324690519</v>
+      </c>
+      <c r="E16" s="1">
+        <v>5.4034018595270403</v>
+      </c>
+      <c r="F16" s="1">
+        <v>6.7187030465282902</v>
+      </c>
+      <c r="G16">
+        <v>4.9910479056059396</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="1">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1">
+        <v>6.80505251417922</v>
+      </c>
+      <c r="C17" s="1">
+        <v>4.7580544023353797</v>
+      </c>
+      <c r="D17" s="1">
+        <v>6.6239507538990798</v>
+      </c>
+      <c r="E17" s="1">
+        <v>6.7876696825845002</v>
+      </c>
+      <c r="F17" s="1">
+        <v>10.572679108768099</v>
+      </c>
+      <c r="G17">
+        <v>5.1657993131130899</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="1">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1">
+        <v>7.0139954817328496</v>
+      </c>
+      <c r="C18" s="1">
+        <v>4.78049755251826</v>
+      </c>
+      <c r="D18" s="1">
+        <v>4.9721128584306804</v>
+      </c>
+      <c r="E18" s="1">
+        <v>7.4162952015033801</v>
+      </c>
+      <c r="F18" s="1">
+        <v>1.6651779764186201</v>
+      </c>
+      <c r="G18">
+        <v>4.5998128253412602</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" s="1">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1">
+        <v>5.5458454174790504</v>
+      </c>
+      <c r="C19" s="1">
+        <v>7.2120121318486001</v>
+      </c>
+      <c r="D19" s="1">
+        <v>4.78403334637005</v>
+      </c>
+      <c r="E19" s="1">
+        <v>9.2947141464366094</v>
+      </c>
+      <c r="F19" s="1">
+        <v>7.2642075916728004</v>
+      </c>
+      <c r="G19">
+        <v>9.5927856026248399</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" s="1">
+        <v>19</v>
+      </c>
+      <c r="B20" s="1">
+        <v>7.0821978453152301</v>
+      </c>
+      <c r="C20" s="1">
+        <v>4.7827261278749997</v>
+      </c>
+      <c r="D20" s="1">
+        <v>5.5918466939976801</v>
+      </c>
+      <c r="E20" s="1">
+        <v>3.51918656100767</v>
+      </c>
+      <c r="F20" s="1">
+        <v>5.0571903671312901</v>
+      </c>
+      <c r="G20">
+        <v>5.3250571026972198</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" s="1">
+        <v>20</v>
+      </c>
+      <c r="B21" s="1">
+        <v>6.61534445704656</v>
+      </c>
+      <c r="C21" s="1">
+        <v>4.8021429018701296</v>
+      </c>
+      <c r="D21" s="1">
+        <v>6.2597181910912898</v>
+      </c>
+      <c r="E21" s="1">
+        <v>5.0593116148849004</v>
+      </c>
+      <c r="F21" s="1">
+        <v>4.7678080651800201</v>
+      </c>
+      <c r="G21">
+        <v>6.4246414975211197</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" s="1">
+        <v>21</v>
+      </c>
+      <c r="B22" s="1">
+        <v>5.2574110570190404</v>
+      </c>
+      <c r="C22" s="1">
+        <v>1.8304638819049801</v>
+      </c>
+      <c r="D22" s="1">
+        <v>4.4973759446919397</v>
+      </c>
+      <c r="E22" s="1">
+        <v>4.3636817568267796</v>
+      </c>
+      <c r="F22" s="1">
+        <v>4.8421136655809196</v>
+      </c>
+      <c r="G22">
+        <v>4.2797879208770704</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23" s="6">
+        <f>AVERAGE(B2:B22)</f>
+        <v>5.637435175939145</v>
+      </c>
+      <c r="C23" s="6">
+        <f>AVERAGE(C2:C22)</f>
+        <v>5.0061691279076319</v>
+      </c>
+      <c r="D23" s="6">
+        <f>AVERAGE(D2:D22)</f>
+        <v>5.3682735868406626</v>
+      </c>
+      <c r="E23" s="6">
+        <f>AVERAGE(E2:E22)</f>
+        <v>5.5669814094355461</v>
+      </c>
+      <c r="F23" s="6">
+        <f>AVERAGE(F2:F22)</f>
+        <v>5.662594498512548</v>
+      </c>
+      <c r="G23" s="6">
+        <f>AVERAGE(G2:G22)</f>
+        <v>5.5508254185618231</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" t="s">
+        <v>12</v>
+      </c>
+      <c r="B24" s="7">
+        <f>_xlfn.STDEV.P(B2:B22)</f>
+        <v>0.97104396967437245</v>
+      </c>
+      <c r="C24" s="7">
+        <f>_xlfn.STDEV.P(C2:C22)</f>
+        <v>2.3106449919426244</v>
+      </c>
+      <c r="D24" s="7">
+        <f>_xlfn.STDEV.P(D2:D22)</f>
+        <v>1.6995787956842026</v>
+      </c>
+      <c r="E24" s="7">
+        <f>_xlfn.STDEV.P(E2:E22)</f>
+        <v>1.5691258217028261</v>
+      </c>
+      <c r="F24" s="7">
+        <f>_xlfn.STDEV.P(F2:F22)</f>
+        <v>2.1781156530165084</v>
+      </c>
+      <c r="G24" s="7">
+        <f>_xlfn.STDEV.P(G2:G22)</f>
+        <v>1.4224290051391641</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="D25" t="s">
+        <v>22</v>
+      </c>
+      <c r="E25" t="s">
+        <v>21</v>
+      </c>
+      <c r="G25" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="D27" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="D28" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="D29" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="G1:J1 B1:C24 E1:E24 D23:D24 F23:G24">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2:E24 B2:C24 D23:D24 F23:G24">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2:E23 B2:C23 D23 F23:G23">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:C23 D23:G23">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:C23 D23">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:E22">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>